<commit_message>
results ss and auc
</commit_message>
<xml_diff>
--- a/results/metrics_ss_unified.xlsx
+++ b/results/metrics_ss_unified.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="229">
   <si>
     <t xml:space="preserve">Unnamed: 0</t>
   </si>
@@ -46,105 +46,441 @@
     <t xml:space="preserve">f1</t>
   </si>
   <si>
+    <t xml:space="preserve">val</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/000011_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">000011_da</t>
   </si>
   <si>
+    <t xml:space="preserve">63,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/000011/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">51,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0003/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">67,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75,5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0001/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">60,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/000033_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">000033_da</t>
   </si>
   <si>
+    <t xml:space="preserve">57,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0003_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">0003_da</t>
   </si>
   <si>
+    <t xml:space="preserve">72,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0009/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/000033/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">69,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0001_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">0001_da</t>
   </si>
   <si>
+    <t xml:space="preserve">70,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79,1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/2/0009_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">0009_da</t>
   </si>
   <si>
+    <t xml:space="preserve">70,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/000011_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">81,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/000011/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">80,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0003/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">74,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0001/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">86,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/000033_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">83,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0003_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">85,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0009/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">85,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/000033/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">84,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0001_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">87,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/3/0009_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">84,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/000011_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">82,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85,2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/000011/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">81,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/0003/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">83,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/0001/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">82,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/000033_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">81,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84,4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/0003_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">9_da</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/0009/metrics_val/metrics.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/000033/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">56,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71,9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/1/0001_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
@@ -154,6 +490,21 @@
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/000011_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">3_da</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/000011/metrics_val/metrics.xlsx</t>
   </si>
   <si>
@@ -169,46 +520,193 @@
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/0003_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">1_da</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/0009/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">68,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/000033/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">78,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/0001_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">39,5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/5/0009_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">76,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/000011_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">033_da</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/000011/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">83,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0003/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">78,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0001/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">82,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/000033_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">80,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0003_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">011_da</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0009/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">79,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/000033/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">79,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76,5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0001_da/metrics_val/metrics.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">79,7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86,1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">../semantic_segmentation/SS_Halimeda/runs/4/0009_da/metrics_val/metrics.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92,6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,1%</t>
   </si>
 </sst>
 </file>
@@ -218,7 +716,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -246,6 +744,13 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -298,13 +803,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,6 +825,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -324,16 +893,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:I51"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,16 +930,37 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>30</v>
@@ -390,10 +980,40 @@
       <c r="I2" s="0" t="n">
         <v>0.869919737381735</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -419,10 +1039,34 @@
       <c r="I3" s="0" t="n">
         <v>0.869780550035945</v>
       </c>
+      <c r="M3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -448,10 +1092,34 @@
       <c r="I4" s="0" t="n">
         <v>0.806110399579866</v>
       </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -477,16 +1145,40 @@
       <c r="I5" s="0" t="n">
         <v>0.858726411245855</v>
       </c>
+      <c r="M5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>50</v>
@@ -506,16 +1198,40 @@
       <c r="I6" s="0" t="n">
         <v>0.880270588005492</v>
       </c>
+      <c r="M6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>66</v>
@@ -535,10 +1251,40 @@
       <c r="I7" s="0" t="n">
         <v>0.807418757883194</v>
       </c>
+      <c r="L7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -564,10 +1310,34 @@
       <c r="I8" s="0" t="n">
         <v>0.773717754282693</v>
       </c>
+      <c r="M8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -593,16 +1363,40 @@
       <c r="I9" s="0" t="n">
         <v>0.888891348051558</v>
       </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>65</v>
@@ -622,16 +1416,40 @@
       <c r="I10" s="0" t="n">
         <v>0.836698208191247</v>
       </c>
+      <c r="M10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
@@ -651,16 +1469,40 @@
       <c r="I11" s="0" t="n">
         <v>0.773717754282693</v>
       </c>
+      <c r="M11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>82</v>
@@ -680,10 +1522,40 @@
       <c r="I12" s="0" t="n">
         <v>0.819457014433572</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -709,10 +1581,34 @@
       <c r="I13" s="0" t="n">
         <v>0.825914322871174</v>
       </c>
+      <c r="M13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -738,10 +1634,34 @@
       <c r="I14" s="0" t="n">
         <v>0.679837365305656</v>
       </c>
+      <c r="M14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -767,16 +1687,40 @@
       <c r="I15" s="0" t="n">
         <v>0.818975726067352</v>
       </c>
+      <c r="M15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>43</v>
@@ -796,16 +1740,40 @@
       <c r="I16" s="0" t="n">
         <v>0.851349496999299</v>
       </c>
+      <c r="M16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -825,10 +1793,40 @@
       <c r="I17" s="0" t="n">
         <v>0.679837365305656</v>
       </c>
+      <c r="L17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="U17" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -854,10 +1852,34 @@
       <c r="I18" s="0" t="n">
         <v>0.679837365305656</v>
       </c>
+      <c r="M18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -883,16 +1905,40 @@
       <c r="I19" s="0" t="n">
         <v>0.86267603613041</v>
       </c>
+      <c r="M19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>102</v>
@@ -912,16 +1958,42 @@
       <c r="I20" s="0" t="n">
         <v>0.748224879517193</v>
       </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="U20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -941,16 +2013,40 @@
       <c r="I21" s="0" t="n">
         <v>0.679837365305656</v>
       </c>
+      <c r="M21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>89</v>
@@ -970,10 +2066,40 @@
       <c r="I22" s="0" t="n">
         <v>0.830419170940388</v>
       </c>
+      <c r="L22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -999,10 +2125,34 @@
       <c r="I23" s="0" t="n">
         <v>0.860001669485873</v>
       </c>
+      <c r="M23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -1028,10 +2178,34 @@
       <c r="I24" s="0" t="n">
         <v>0.765616383263211</v>
       </c>
+      <c r="M24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="T24" s="0" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -1057,16 +2231,40 @@
       <c r="I25" s="0" t="n">
         <v>0.795601077057566</v>
       </c>
+      <c r="M25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="T25" s="0" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>142</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>61</v>
@@ -1086,16 +2284,40 @@
       <c r="I26" s="0" t="n">
         <v>0.852220817795369</v>
       </c>
+      <c r="M26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="T26" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -1115,10 +2337,40 @@
       <c r="I27" s="0" t="n">
         <v>0.718815195992935</v>
       </c>
+      <c r="L27" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="U27" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -1144,10 +2396,34 @@
       <c r="I28" s="0" t="n">
         <v>0.75498469486762</v>
       </c>
+      <c r="M28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T28" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -1173,16 +2449,40 @@
       <c r="I29" s="0" t="n">
         <v>0.868273060123741</v>
       </c>
+      <c r="M29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="R29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T29" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>97</v>
@@ -1202,16 +2502,40 @@
       <c r="I30" s="0" t="n">
         <v>0.826467641244157</v>
       </c>
+      <c r="M30" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T30" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -1231,16 +2555,40 @@
       <c r="I31" s="0" t="n">
         <v>0.718815195992935</v>
       </c>
+      <c r="M31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T31" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>61</v>
@@ -1260,10 +2608,40 @@
       <c r="I32" s="0" t="n">
         <v>0.861082542737041</v>
       </c>
+      <c r="L32" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="P32" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q32" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="R32" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="S32" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="T32" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="U32" s="0" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -1289,10 +2667,34 @@
       <c r="I33" s="0" t="n">
         <v>0.861712393037971</v>
       </c>
+      <c r="M33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T33" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -1318,10 +2720,34 @@
       <c r="I34" s="0" t="n">
         <v>0.790579159814726</v>
       </c>
+      <c r="M34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q34" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T34" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -1347,16 +2773,40 @@
       <c r="I35" s="0" t="n">
         <v>0.895842984586502</v>
       </c>
+      <c r="M35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q35" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T35" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>55</v>
@@ -1376,16 +2826,40 @@
       <c r="I36" s="0" t="n">
         <v>0.876247633007231</v>
       </c>
+      <c r="M36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="R36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T36" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
@@ -1405,10 +2879,40 @@
       <c r="I37" s="0" t="n">
         <v>0.749764254011243</v>
       </c>
+      <c r="L37" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="P37" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q37" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="R37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="T37" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="U37" s="0" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -1434,10 +2938,34 @@
       <c r="I38" s="0" t="n">
         <v>0.749764254011243</v>
       </c>
+      <c r="M38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N38" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="R38" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="T38" s="0" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -1463,16 +2991,40 @@
       <c r="I39" s="0" t="n">
         <v>0.898545325007201</v>
       </c>
+      <c r="M39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="R39" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="T39" s="0" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>179</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>71</v>
@@ -1492,16 +3044,40 @@
       <c r="I40" s="0" t="n">
         <v>0.844474473976132</v>
       </c>
+      <c r="M40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="R40" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="T40" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0</v>
@@ -1521,16 +3097,40 @@
       <c r="I41" s="0" t="n">
         <v>0.749764254011243</v>
       </c>
+      <c r="M41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="R41" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="T41" s="0" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>46</v>
@@ -1550,10 +3150,40 @@
       <c r="I42" s="0" t="n">
         <v>0.844917597474913</v>
       </c>
+      <c r="L42" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N42" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="R42" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="T42" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="U42" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -1579,10 +3209,34 @@
       <c r="I43" s="0" t="n">
         <v>0.844407937056205</v>
       </c>
+      <c r="M43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="R43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="T43" s="0" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -1608,10 +3262,34 @@
       <c r="I44" s="0" t="n">
         <v>0.778039506119271</v>
       </c>
+      <c r="M44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q44" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="R44" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="S44" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="T44" s="0" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>56</v>
+        <v>199</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -1637,16 +3315,40 @@
       <c r="I45" s="0" t="n">
         <v>0.865526925208999</v>
       </c>
+      <c r="M45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N45" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q45" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="R45" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="S45" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="T45" s="0" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>35</v>
@@ -1666,16 +3368,40 @@
       <c r="I46" s="0" t="n">
         <v>0.83656118787392</v>
       </c>
+      <c r="M46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N46" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q46" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="R46" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="S46" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="T46" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>207</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>0</v>
@@ -1695,10 +3421,40 @@
       <c r="I47" s="0" t="n">
         <v>0.730796481548649</v>
       </c>
+      <c r="L47" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="P47" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q47" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="R47" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="S47" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="T47" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="U47" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -1724,10 +3480,34 @@
       <c r="I48" s="0" t="n">
         <v>0.730796481548649</v>
       </c>
+      <c r="M48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="P48" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q48" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="R48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="T48" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>60</v>
+        <v>215</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -1753,16 +3533,40 @@
       <c r="I49" s="0" t="n">
         <v>0.872130194469578</v>
       </c>
+      <c r="M49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="R49" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="S49" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="T49" s="0" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>56</v>
@@ -1782,16 +3586,40 @@
       <c r="I50" s="0" t="n">
         <v>0.833648461969806</v>
       </c>
+      <c r="M50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q50" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="R50" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="T50" s="0" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>225</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
@@ -1811,7 +3639,32 @@
       <c r="I51" s="0" t="n">
         <v>0.730796481548649</v>
       </c>
-    </row>
+      <c r="M51" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="P51" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q51" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="R51" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="S51" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="T51" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>